<commit_message>
entered course eval data math w16
Started in a .xlsx file but then made a new .xlsm, still gotta make sure that format works with what's been done so far
</commit_message>
<xml_diff>
--- a/W16_Math.xlsx
+++ b/W16_Math.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eloisechakour/Desktop/B21_Research/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ppest\OneDrive\Documents\GitHub\B21Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8A9313EBA0A1F9512081C9D78789E539E63AEF62" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="460" windowWidth="28160" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -77,7 +78,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -124,6 +125,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -391,14 +395,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
@@ -413,12 +417,12 @@
     <col min="13" max="13" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
@@ -433,7 +437,7 @@
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -474,7 +478,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>111</v>
       </c>
@@ -519,7 +523,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>122</v>
       </c>
@@ -564,7 +568,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" s="2">
         <v>123</v>
       </c>
@@ -609,7 +613,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B7" s="2">
         <v>123</v>
       </c>
@@ -654,7 +658,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B8" s="2">
         <v>133</v>
       </c>
@@ -699,7 +703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>140</v>
       </c>
@@ -744,7 +748,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>141</v>
       </c>
@@ -789,7 +793,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B11" s="2">
         <v>141</v>
       </c>
@@ -834,7 +838,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B12" s="2">
         <v>151</v>
       </c>
@@ -879,7 +883,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B13" s="2">
         <v>203</v>
       </c>
@@ -924,7 +928,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B14" s="2">
         <v>203</v>
       </c>
@@ -969,7 +973,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" s="2">
         <v>204</v>
       </c>
@@ -1014,7 +1018,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>204</v>
       </c>
@@ -1059,7 +1063,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="2">
         <v>222</v>
       </c>
@@ -1104,7 +1108,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" s="2">
         <v>223</v>
       </c>
@@ -1149,7 +1153,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" s="2">
         <v>236</v>
       </c>
@@ -1194,7 +1198,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>243</v>
       </c>
@@ -1239,7 +1243,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" s="2">
         <v>243</v>
       </c>
@@ -1284,7 +1288,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B22" s="2">
         <v>247</v>
       </c>
@@ -1329,7 +1333,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B23" s="2">
         <v>249</v>
       </c>
@@ -1374,7 +1378,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>251</v>
       </c>
@@ -1419,7 +1423,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B25" s="2">
         <v>255</v>
       </c>
@@ -1464,7 +1468,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B26" s="2">
         <v>314</v>
       </c>
@@ -1509,7 +1513,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B27" s="2">
         <v>315</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B28" s="2">
         <v>319</v>
       </c>
@@ -1599,7 +1603,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B29" s="2">
         <v>323</v>
       </c>
@@ -1644,7 +1648,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B30" s="2">
         <v>324</v>
       </c>
@@ -1689,7 +1693,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B31" s="2">
         <v>325</v>
       </c>
@@ -1734,7 +1738,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B32" s="2">
         <v>329</v>
       </c>
@@ -1779,7 +1783,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B33" s="2">
         <v>340</v>
       </c>
@@ -1824,7 +1828,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B34" s="2">
         <v>357</v>
       </c>
@@ -1869,7 +1873,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B35" s="2">
         <v>387</v>
       </c>
@@ -1914,7 +1918,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B36" s="2">
         <v>430</v>
       </c>
@@ -1959,7 +1963,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B37" s="2">
         <v>437</v>
       </c>
@@ -2004,7 +2008,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B38" s="2">
         <v>447</v>
       </c>
@@ -2049,7 +2053,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B39" s="2">
         <v>455</v>
       </c>
@@ -2094,7 +2098,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B40" s="2">
         <v>457</v>
       </c>
@@ -2139,7 +2143,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B41" s="2">
         <v>458</v>
       </c>
@@ -2184,7 +2188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B42" s="2">
         <v>523</v>
       </c>
@@ -2229,7 +2233,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B43" s="2">
         <v>537</v>
       </c>
@@ -2274,7 +2278,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B44" s="2">
         <v>540</v>
       </c>
@@ -2319,7 +2323,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B45" s="2">
         <v>550</v>
       </c>
@@ -2364,7 +2368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B46" s="2">
         <v>552</v>
       </c>
@@ -2409,7 +2413,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B47" s="2">
         <v>557</v>
       </c>
@@ -2454,7 +2458,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B48" s="2">
         <v>565</v>
       </c>
@@ -2499,7 +2503,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B49" s="2">
         <v>566</v>
       </c>
@@ -2544,7 +2548,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B50" s="2">
         <v>571</v>
       </c>
@@ -2589,7 +2593,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B51" s="2">
         <v>577</v>
       </c>
@@ -2634,7 +2638,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="52" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B52" s="2">
         <v>579</v>
       </c>
@@ -2679,7 +2683,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="53" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B53" s="2">
         <v>591</v>
       </c>
@@ -2724,7 +2728,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="2:15" x14ac:dyDescent="0.2">
+    <row r="54" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B54" s="2">
         <v>596</v>
       </c>

</xml_diff>